<commit_message>
atualizei dados da BIBI
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/estatisticas_faturamento_diario.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/estatisticas_faturamento_diario.xlsx
@@ -426,13 +426,13 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1077628.61</v>
+        <v>587582.36</v>
       </c>
       <c r="C2">
-        <v>35920.95366666667</v>
+        <v>19586.07866666666</v>
       </c>
       <c r="D2">
-        <v>127489.8</v>
+        <v>31800.92</v>
       </c>
       <c r="E2">
         <v>16</v>
@@ -443,13 +443,13 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>941184.13</v>
+        <v>763210.77</v>
       </c>
       <c r="C3">
-        <v>33613.71892857143</v>
+        <v>27257.5275</v>
       </c>
       <c r="D3">
-        <v>110712.73</v>
+        <v>57356.01</v>
       </c>
       <c r="E3">
         <v>17</v>
@@ -460,16 +460,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>796983.15</v>
+        <v>670620.61</v>
       </c>
       <c r="C4">
-        <v>25709.13387096774</v>
+        <v>21632.9229032258</v>
       </c>
       <c r="D4">
-        <v>65503.24</v>
+        <v>51663.12</v>
       </c>
       <c r="E4">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -477,16 +477,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>610425.76</v>
+        <v>511614.46</v>
       </c>
       <c r="C5">
-        <v>25434.40666666667</v>
+        <v>18271.945</v>
       </c>
       <c r="D5">
-        <v>99475.81</v>
+        <v>38515.34</v>
       </c>
       <c r="E5">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>